<commit_message>
Invoice Product Info Printing Help needed
I still have troubles with printing product information in the invoice. How about we make Product items first?
</commit_message>
<xml_diff>
--- a/Customer_List.xlsx
+++ b/Customer_List.xlsx
@@ -1,36 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mslaw\eclipse-workspace\Assignment-3 Github Folder\ReadCSVExamples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3bc697bdb8b8b24/Documents/University Documents/CSULB Documents/CSULB CECS Files/CECS 543 Software Engineering/Assignments/Assignment 3/Assignment-3 Github Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59E53B87-086B-42C6-9101-D45FCC2E8A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75501E16-A28D-45CB-8A79-40050E7FFD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{07FB71F9-5D30-426A-9F44-0BE171535884}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -52,56 +37,56 @@
     <t>Sales Tax %</t>
   </si>
   <si>
+    <t>Meiling Gonzalez</t>
+  </si>
+  <si>
+    <t>5555 Campo Walk; Long Beach; CA; 90803</t>
+  </si>
+  <si>
     <t>(562)123-4567</t>
   </si>
   <si>
     <t>Justin Marsh</t>
   </si>
   <si>
+    <t>8989 Speilberg Ave; Hollywood; CA; 90028</t>
+  </si>
+  <si>
     <t>(323)515-0708</t>
   </si>
   <si>
     <t>Jamal Zhao</t>
   </si>
   <si>
+    <t>1234 Goldenwest Ave; Huntington Beach; CA; 92605</t>
+  </si>
+  <si>
     <t>(714)987-6543</t>
   </si>
   <si>
-    <t>Meiling Gonzalez</t>
-  </si>
-  <si>
     <t>Miguel Diep</t>
   </si>
   <si>
+    <t>14345 South St; Cerritos; CA; 90703</t>
+  </si>
+  <si>
     <t>(562)128-1111</t>
   </si>
   <si>
     <t>Maria Booker</t>
   </si>
   <si>
+    <t>1234 Garvey Ave; San Gabriel; CA; 91776</t>
+  </si>
+  <si>
     <t>(626)108-1215</t>
-  </si>
-  <si>
-    <t>5555 Campo Walk; Long Beach; CA; 90803</t>
-  </si>
-  <si>
-    <t>8989 Speilberg Ave; Hollywood; CA; 90028</t>
-  </si>
-  <si>
-    <t>1234 Goldenwest Ave; Huntington Beach; CA; 92605</t>
-  </si>
-  <si>
-    <t>14345 South St; Cerritos; CA; 90703</t>
-  </si>
-  <si>
-    <t>1234 Garvey Ave; San Gabriel; CA; 91776</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,16 +94,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -126,17 +411,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,18 +919,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993930CD-4D3F-4870-9987-B37D4D2FAADF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,16 +957,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.105</v>
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>10.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -502,16 +974,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>9.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -519,16 +991,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7.7499999999999999E-2</v>
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>7.75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -536,16 +1008,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -553,16 +1025,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.06</v>
+      <c r="E6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating and printing the Invoice is 90% done! :)
I'm almost done with creating the Invoice, calculating its amount, and printing it to the console. The program already creates and prints an invoice in a neat format! All we need to do is add the delivery charge, the dates, and a few other things and we will be done with creating the invoice! :+1:
</commit_message>
<xml_diff>
--- a/Customer_List.xlsx
+++ b/Customer_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3bc697bdb8b8b24/Documents/University Documents/CSULB Documents/CSULB CECS Files/CECS 543 Software Engineering/Assignments/Assignment 3/Assignment-3 Github Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75501E16-A28D-45CB-8A79-40050E7FFD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{E309CF12-1476-4CC3-81EB-792D86CF7EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Customer_List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Customer ID</t>
   </si>
@@ -43,43 +44,28 @@
     <t>5555 Campo Walk; Long Beach; CA; 90803</t>
   </si>
   <si>
-    <t>(562)123-4567</t>
-  </si>
-  <si>
     <t>Justin Marsh</t>
   </si>
   <si>
     <t>8989 Speilberg Ave; Hollywood; CA; 90028</t>
   </si>
   <si>
-    <t>(323)515-0708</t>
-  </si>
-  <si>
     <t>Jamal Zhao</t>
   </si>
   <si>
     <t>1234 Goldenwest Ave; Huntington Beach; CA; 92605</t>
   </si>
   <si>
-    <t>(714)987-6543</t>
-  </si>
-  <si>
     <t>Miguel Diep</t>
   </si>
   <si>
     <t>14345 South St; Cerritos; CA; 90703</t>
   </si>
   <si>
-    <t>(562)128-1111</t>
-  </si>
-  <si>
     <t>Maria Booker</t>
   </si>
   <si>
     <t>1234 Garvey Ave; San Gabriel; CA; 91776</t>
-  </si>
-  <si>
-    <t>(626)108-1215</t>
   </si>
 </sst>
 </file>
@@ -923,7 +909,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -932,7 +918,6 @@
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -962,8 +947,8 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>1621234567</v>
       </c>
       <c r="E2">
         <v>10.5</v>
@@ -974,13 +959,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="D3">
+        <v>1235150708</v>
       </c>
       <c r="E3">
         <v>9.5</v>
@@ -991,13 +976,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1149876543</v>
       </c>
       <c r="E4">
         <v>7.75</v>
@@ -1008,13 +993,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1621281111</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -1025,13 +1010,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1261081215</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -1039,6 +1024,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>